<commit_message>
add opencsv to general bean
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -99,6 +99,18 @@
   </si>
   <si>
     <t>Date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>日期list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>List&lt;Integer&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -432,7 +444,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
@@ -440,79 +452,88 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F3" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G3" t="s">
         <v>16</v>
       </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -532,6 +553,9 @@
         <v>123</v>
       </c>
       <c r="G4" s="1">
+        <v>43739</v>
+      </c>
+      <c r="H4" s="1">
         <v>43739</v>
       </c>
     </row>

</xml_diff>